<commit_message>
Recoupmentplan vorläufig ausgefüllt. Erloesvorschau die Stückzahl bei Anzu von der Gesamtsumme ausgeschlossen.
</commit_message>
<xml_diff>
--- a/Produktionsförderung/Anlage_6_Vorlage_Recoupmentplan_GBW.xlsx
+++ b/Produktionsförderung/Anlage_6_Vorlage_Recoupmentplan_GBW.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\ScrewDriversMFG\Produktionsförderung\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78E7BA6C-4430-4268-800A-B56F411DA527}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B212C849-7DCF-438B-BC1B-661461233FE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="77040" windowHeight="31920" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28695" yWindow="0" windowWidth="29010" windowHeight="31785" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Vorlage" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="29">
   <si>
     <t>Beteiligte</t>
   </si>
@@ -81,9 +81,6 @@
     <t>weitere benötigte Posten bitte ergänzen, bzw. nicht Benötigtes Löschen</t>
   </si>
   <si>
-    <t>(eigene Rückstellungen</t>
-  </si>
-  <si>
     <t>eigene Rückstellungen Antragsteller</t>
   </si>
   <si>
@@ -118,6 +115,15 @@
   </si>
   <si>
     <t>Rückstellungen MFG</t>
+  </si>
+  <si>
+    <t>(eigene Rückstellungen)</t>
+  </si>
+  <si>
+    <t>Gesamtprojektkosten</t>
+  </si>
+  <si>
+    <t>Eigenanteil</t>
   </si>
 </sst>
 </file>
@@ -130,7 +136,7 @@
     <numFmt numFmtId="164" formatCode="_-* #,##0\ [$€-407]_-;\-* #,##0\ [$€-407]_-;_-* &quot;-&quot;??\ [$€-407]_-;_-@_-"/>
     <numFmt numFmtId="165" formatCode="_-* #,##0\ &quot;€&quot;_-;\-* #,##0\ &quot;€&quot;_-;_-* &quot;-&quot;??\ &quot;€&quot;_-;_-@_-"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -168,6 +174,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -831,7 +844,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="72">
+  <cellXfs count="73">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
@@ -1026,18 +1039,19 @@
     <xf numFmtId="10" fontId="2" fillId="3" borderId="10" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="44" fontId="2" fillId="2" borderId="29" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="28" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="30" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="2" fillId="2" borderId="29" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="2" fillId="0" borderId="28" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="2" fillId="0" borderId="30" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
+    <xf numFmtId="44" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Prozent" xfId="2" builtinId="5"/>
@@ -1372,18 +1386,18 @@
   <sheetPr>
     <tabColor theme="9" tint="0.79998168889431442"/>
   </sheetPr>
-  <dimension ref="A1:G27"/>
+  <dimension ref="A1:G30"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" zoomScale="175" zoomScaleNormal="100" zoomScalePageLayoutView="175" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+    <sheetView tabSelected="1" view="pageLayout" zoomScale="115" zoomScaleNormal="100" zoomScalePageLayoutView="115" workbookViewId="0">
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="33.42578125" customWidth="1"/>
-    <col min="2" max="2" width="13" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.28515625" style="3" customWidth="1"/>
-    <col min="4" max="4" width="13" style="1" customWidth="1"/>
+    <col min="4" max="4" width="14" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.5703125" customWidth="1"/>
     <col min="7" max="7" width="13.140625" style="2" customWidth="1"/>
   </cols>
@@ -1417,13 +1431,15 @@
         <v>9</v>
       </c>
       <c r="D3" s="26">
-        <v>0</v>
+        <f>B9</f>
+        <v>309333.14</v>
       </c>
       <c r="E3" s="66" t="s">
         <v>9</v>
       </c>
       <c r="F3" s="26">
-        <v>0</v>
+        <f>B9+D13</f>
+        <v>453621.5</v>
       </c>
       <c r="G3" s="64" t="s">
         <v>9</v>
@@ -1434,11 +1450,13 @@
         <v>5</v>
       </c>
       <c r="B4" s="9">
-        <v>0</v>
+        <f>B6</f>
+        <v>309333.14</v>
       </c>
       <c r="C4" s="67"/>
       <c r="D4" s="27">
-        <v>0</v>
+        <f>D3+D10+D11</f>
+        <v>453621.5</v>
       </c>
       <c r="E4" s="67"/>
       <c r="F4" s="20"/>
@@ -1446,7 +1464,7 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="36" t="s">
-        <v>14</v>
+        <v>26</v>
       </c>
       <c r="B5" s="6">
         <v>0</v>
@@ -1461,13 +1479,13 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="37" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B6" s="7">
         <v>309333.14</v>
       </c>
       <c r="C6" s="10">
-        <v>0.2</v>
+        <v>1</v>
       </c>
       <c r="D6" s="60"/>
       <c r="E6" s="61"/>
@@ -1527,10 +1545,12 @@
       <c r="B10" s="56"/>
       <c r="C10" s="57"/>
       <c r="D10" s="13">
-        <v>127999.92</v>
+        <f>B29/2</f>
+        <v>131171.24</v>
       </c>
       <c r="E10" s="21">
-        <v>0</v>
+        <f>1-E11</f>
+        <v>0.90000003049448951</v>
       </c>
       <c r="F10" s="60"/>
       <c r="G10" s="63"/>
@@ -1542,10 +1562,11 @@
       <c r="B11" s="53"/>
       <c r="C11" s="54"/>
       <c r="D11" s="14">
-        <v>0</v>
+        <v>13117.12</v>
       </c>
       <c r="E11" s="15">
-        <v>0</v>
+        <f>D11/D10</f>
+        <v>9.9999969505510516E-2</v>
       </c>
       <c r="F11" s="60"/>
       <c r="G11" s="63"/>
@@ -1573,7 +1594,7 @@
       <c r="C13" s="51"/>
       <c r="D13" s="18">
         <f>SUM(D10:D12)</f>
-        <v>127999.92</v>
+        <v>144288.35999999999</v>
       </c>
       <c r="E13" s="19">
         <v>1</v>
@@ -1601,7 +1622,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
@@ -1615,20 +1636,37 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>25</v>
-      </c>
-      <c r="B26" s="1">
+        <v>24</v>
+      </c>
+      <c r="B26" s="72">
         <f>10666.66*(8+9)+10666.66*12</f>
         <v>309333.14</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>26</v>
-      </c>
-      <c r="B27" s="1">
+        <v>25</v>
+      </c>
+      <c r="B27" s="72">
         <f>10666.66*12</f>
         <v>127999.92</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>27</v>
+      </c>
+      <c r="B29" s="72">
+        <v>262342.48</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>28</v>
+      </c>
+      <c r="B30" s="72">
+        <f>0.05*B29</f>
+        <v>13117.124</v>
       </c>
     </row>
   </sheetData>
@@ -1692,7 +1730,7 @@
       <c r="D2" s="47" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="69"/>
+      <c r="E2" s="68"/>
       <c r="F2" s="45" t="s">
         <v>3</v>
       </c>
@@ -1738,7 +1776,7 @@
     </row>
     <row r="5" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="33" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B5" s="13">
         <v>10000</v>
@@ -1768,7 +1806,7 @@
     </row>
     <row r="7" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="35" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B7" s="28">
         <v>10000</v>
@@ -1814,7 +1852,7 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="52" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B10" s="53"/>
       <c r="C10" s="54"/>
@@ -1829,7 +1867,7 @@
     </row>
     <row r="11" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="52" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B11" s="53"/>
       <c r="C11" s="54"/>
@@ -1866,51 +1904,51 @@
       <c r="C13" s="41"/>
       <c r="D13" s="41"/>
       <c r="E13" s="42"/>
-      <c r="F13" s="70">
+      <c r="F13" s="69">
         <v>1</v>
       </c>
-      <c r="G13" s="71"/>
+      <c r="G13" s="70"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="29" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="71" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="68" t="s">
+      <c r="B16" s="71"/>
+      <c r="C16" s="71"/>
+      <c r="D16" s="71"/>
+      <c r="E16" s="71"/>
+      <c r="F16" s="71"/>
+      <c r="G16" s="71"/>
+      <c r="H16" s="71"/>
+    </row>
+    <row r="17" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="71" t="s">
         <v>20</v>
       </c>
-      <c r="B16" s="68"/>
-      <c r="C16" s="68"/>
-      <c r="D16" s="68"/>
-      <c r="E16" s="68"/>
-      <c r="F16" s="68"/>
-      <c r="G16" s="68"/>
-      <c r="H16" s="68"/>
-    </row>
-    <row r="17" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="68" t="s">
+      <c r="B17" s="71"/>
+      <c r="C17" s="71"/>
+      <c r="D17" s="71"/>
+      <c r="E17" s="71"/>
+      <c r="F17" s="71"/>
+      <c r="G17" s="71"/>
+      <c r="H17" s="71"/>
+    </row>
+    <row r="18" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="71" t="s">
         <v>21</v>
       </c>
-      <c r="B17" s="68"/>
-      <c r="C17" s="68"/>
-      <c r="D17" s="68"/>
-      <c r="E17" s="68"/>
-      <c r="F17" s="68"/>
-      <c r="G17" s="68"/>
-      <c r="H17" s="68"/>
-    </row>
-    <row r="18" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="68" t="s">
-        <v>22</v>
-      </c>
-      <c r="B18" s="68"/>
-      <c r="C18" s="68"/>
-      <c r="D18" s="68"/>
-      <c r="E18" s="68"/>
-      <c r="F18" s="68"/>
-      <c r="G18" s="68"/>
-      <c r="H18" s="68"/>
+      <c r="B18" s="71"/>
+      <c r="C18" s="71"/>
+      <c r="D18" s="71"/>
+      <c r="E18" s="71"/>
+      <c r="F18" s="71"/>
+      <c r="G18" s="71"/>
+      <c r="H18" s="71"/>
     </row>
     <row r="19" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="4"/>
@@ -1921,6 +1959,14 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="A16:H16"/>
+    <mergeCell ref="A17:H17"/>
+    <mergeCell ref="A18:H18"/>
+    <mergeCell ref="A9:C9"/>
+    <mergeCell ref="A10:C10"/>
+    <mergeCell ref="A11:C11"/>
+    <mergeCell ref="A12:C12"/>
+    <mergeCell ref="A13:E13"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="D2:E2"/>
     <mergeCell ref="F2:G2"/>
@@ -1930,14 +1976,6 @@
     <mergeCell ref="G3:G4"/>
     <mergeCell ref="D5:E8"/>
     <mergeCell ref="F5:G12"/>
-    <mergeCell ref="A16:H16"/>
-    <mergeCell ref="A17:H17"/>
-    <mergeCell ref="A18:H18"/>
-    <mergeCell ref="A9:C9"/>
-    <mergeCell ref="A10:C10"/>
-    <mergeCell ref="A11:C11"/>
-    <mergeCell ref="A12:C12"/>
-    <mergeCell ref="A13:E13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>